<commit_message>
Re valoracion del proceso
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Beecker\Documents\UiPath\LIV-CP\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD60BCB-2149-49E2-BDB3-11BBF6F1A36C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E5D428-5E67-4A4A-B7C6-1C4D2951BC06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="104">
   <si>
     <t>Name</t>
   </si>
@@ -271,7 +271,79 @@
     <t>Pruebas</t>
   </si>
   <si>
-    <t>S4HANA SUBURBIA</t>
+    <t>DIP2-FI-1</t>
+  </si>
+  <si>
+    <t>SAP</t>
+  </si>
+  <si>
+    <t>Contrasena</t>
+  </si>
+  <si>
+    <t>Productivo2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S4HANA SUBURBIA SBP </t>
+  </si>
+  <si>
+    <t>KeyPath</t>
+  </si>
+  <si>
+    <t>C:\Users\Beecker\Documents\Liverpool\Coneccion Google\uipath-test-256814-4eff096b6385_Proveedor.json</t>
+  </si>
+  <si>
+    <t>IDAccount</t>
+  </si>
+  <si>
+    <t>notasecret</t>
+  </si>
+  <si>
+    <t>uipathproveedor@uipath-test-256814.iam.gserviceaccount.com</t>
+  </si>
+  <si>
+    <t>Secret</t>
+  </si>
+  <si>
+    <t>NombreArchivo</t>
+  </si>
+  <si>
+    <t>Carta Porte</t>
+  </si>
+  <si>
+    <t>IdCarpetaPadre</t>
+  </si>
+  <si>
+    <t>1GboE8jWrN6EmQCZl6VlMmwdrqe_4k9kJ</t>
+  </si>
+  <si>
+    <t>RutaDescargaTemporal</t>
+  </si>
+  <si>
+    <t>Data\Temporal\Carta Porte</t>
+  </si>
+  <si>
+    <t>RutaProveedoresXLSX</t>
+  </si>
+  <si>
+    <t>RutaProveedoresCSV</t>
+  </si>
+  <si>
+    <t>C:\Users\Beecker\Documents\UiPath\LIV-CP\Data\Proveedores\Proveedores.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\Beecker\Documents\UiPath\LIV-CP\Data\Proveedores\Proveedores.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\Beecker\Documents\UiPath\LIV-CP\Data\Log\</t>
+  </si>
+  <si>
+    <t>RutaLog</t>
+  </si>
+  <si>
+    <t>C:\Users\Beecker\Documents\UiPath\LIV-CP\Data\Extras\Plantilla Log.xlsx</t>
+  </si>
+  <si>
+    <t>PlantillaLogRuta</t>
   </si>
 </sst>
 </file>
@@ -374,7 +446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
@@ -405,6 +477,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -721,8 +794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1038"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="49.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -802,7 +875,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>5</v>
@@ -900,8 +973,12 @@
       <c r="Z5"/>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6"/>
-      <c r="B6" s="6"/>
+      <c r="A6" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>79</v>
+      </c>
       <c r="C6"/>
       <c r="D6"/>
       <c r="E6"/>
@@ -928,8 +1005,12 @@
       <c r="Z6"/>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7"/>
-      <c r="B7" s="6"/>
+      <c r="A7" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>82</v>
+      </c>
       <c r="C7"/>
       <c r="D7"/>
       <c r="E7"/>
@@ -956,7 +1037,6 @@
       <c r="Z7"/>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8"/>
       <c r="B8" s="6"/>
       <c r="C8"/>
       <c r="D8"/>
@@ -2882,14 +2962,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" style="8" customWidth="1"/>
-    <col min="2" max="2" width="50.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.5546875" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="80.33203125" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="26" width="8.6640625" style="8" customWidth="1"/>
     <col min="27" max="27" width="14.44140625" style="8" customWidth="1"/>
@@ -3139,14 +3219,86 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="1" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:3" s="1" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:3" s="1" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:3" s="1" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:3" s="1" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:3" s="1" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:3" s="1" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:3" s="1" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:3" ht="15" customHeight="1">
+      <c r="A21" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15" customHeight="1">
+      <c r="A22" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" s="1" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A23" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" s="1" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A24" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" s="1" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A25" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" s="1" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A26" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" s="1" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A27" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" s="1" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A28" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" s="1" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A29" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" s="1" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A30" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
     <row r="31" spans="1:3" s="1" customFormat="1" ht="14.25" customHeight="1"/>
     <row r="32" spans="1:3" s="1" customFormat="1" ht="14.25" customHeight="1"/>
     <row r="33" spans="3:3" s="1" customFormat="1" ht="14.25" customHeight="1">

</xml_diff>